<commit_message>
Correct endo-learn/SYSoCCtaSC input data to use decimal format
</commit_message>
<xml_diff>
--- a/InputData/endo-learn/SYSoCCtaSC/Start Yr Shares of Capacity Costs that are Soft Costs.xlsx
+++ b/InputData/endo-learn/SYSoCCtaSC/Start Yr Shares of Capacity Costs that are Soft Costs.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jeff-nonadmin\CodeRepositories\eps-us\InputData\endo-learn\SYSoCCtaSC\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F4D2AA02-27FC-41E2-A128-5F9185E7D892}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{36812C60-10F4-471D-A279-B5D2C888C3D9}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3735" yWindow="405" windowWidth="24435" windowHeight="16275" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2145" yWindow="285" windowWidth="22170" windowHeight="16110" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="About" sheetId="1" r:id="rId1"/>
@@ -1492,7 +1492,7 @@
       <c r="A2" t="s">
         <v>81</v>
       </c>
-      <c r="B2" s="3">
+      <c r="B2" s="13">
         <f>AVERAGE(Data!B64:B65)</f>
         <v>0.63500000000000001</v>
       </c>

</xml_diff>

<commit_message>
Partition labor, foreign entities, and government shares of nonenergy industry revenue on Cumulators sheet, after summing across sectors.  Partition labor (and taxes on labor) shares of energy industry revenue similarly.  We continue to handle most fuel taxes within the sectors and to handle foreign entities' share of energy industry revenue in energy import/export code on the Fuels sheet.  Note that this commit is an intermediate stage of model development that requires updates to the IO Model and to the Cost Outputs calculations. (#66)
</commit_message>
<xml_diff>
--- a/InputData/endo-learn/SYSoCCtaSC/Start Yr Shares of Capacity Costs that are Soft Costs.xlsx
+++ b/InputData/endo-learn/SYSoCCtaSC/Start Yr Shares of Capacity Costs that are Soft Costs.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22624"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22827"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jeff-nonadmin\CodeRepositories\eps-us\InputData\endo-learn\SYSoCCtaSC\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{36812C60-10F4-471D-A279-B5D2C888C3D9}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{441BA37F-16B0-4405-B919-798EEE889669}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2145" yWindow="285" windowWidth="22170" windowHeight="16110" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="About" sheetId="1" r:id="rId1"/>
@@ -18,7 +18,7 @@
     <sheet name="SYSoCCtaSC-electricity" sheetId="2" r:id="rId3"/>
     <sheet name="SYSoCCtaSC-buildings" sheetId="5" r:id="rId4"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="191029" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="116" uniqueCount="83">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="117" uniqueCount="84">
   <si>
     <t>Sources:</t>
   </si>
@@ -263,9 +263,6 @@
     <t>offshore wind</t>
   </si>
   <si>
-    <t>Data in this variable are only used for onshore wind, offshore wind, and solar PV.</t>
-  </si>
-  <si>
     <t>SYSoCCtaSC Start Year Shares of Capacity Costs that are Soft Costs</t>
   </si>
   <si>
@@ -284,7 +281,13 @@
     <t>distributed solar</t>
   </si>
   <si>
-    <t>SYSoCCtaSC Share of Distributed Solar and Retrofitting Costs that is Labor</t>
+    <t>Data in this variable are only used for onshore wind, offshore wind, and solar PV</t>
+  </si>
+  <si>
+    <t>(as well as distributed solar).</t>
+  </si>
+  <si>
+    <t>SYSoCCtaSC Start Year Share of Distributed Solar Costs that are Soft Costs</t>
   </si>
 </sst>
 </file>
@@ -665,7 +668,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B37"/>
+  <dimension ref="A1:B38"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -676,12 +679,12 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
@@ -779,51 +782,56 @@
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A27" t="s">
-        <v>53</v>
+        <v>81</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>82</v>
       </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
         <v>55</v>
-      </c>
-    </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A31" t="s">
-        <v>56</v>
       </c>
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="33" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="34" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
         <v>58</v>
-      </c>
-    </row>
-    <row r="35" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A35" t="s">
-        <v>59</v>
       </c>
     </row>
     <row r="36" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="37" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="38" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A38" t="s">
         <v>61</v>
       </c>
     </row>
@@ -1326,7 +1334,7 @@
   <sheetData>
     <row r="1" spans="1:2" ht="45" x14ac:dyDescent="0.25">
       <c r="B1" s="15" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
@@ -1438,7 +1446,7 @@
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B15">
         <f>B11</f>
@@ -1447,7 +1455,7 @@
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B16">
         <f>B11</f>
@@ -1456,7 +1464,7 @@
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B17">
         <f>B9</f>
@@ -1485,12 +1493,12 @@
   <sheetData>
     <row r="1" spans="1:2" ht="45" x14ac:dyDescent="0.25">
       <c r="B1" s="15" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B2" s="13">
         <f>AVERAGE(Data!B64:B65)</f>

</xml_diff>

<commit_message>
Start year updates to 2018 SYC, SYSoCCta, BAADTbVT
</commit_message>
<xml_diff>
--- a/InputData/endo-learn/SYSoCCtaSC/Start Yr Shares of Capacity Costs that are Soft Costs.xlsx
+++ b/InputData/endo-learn/SYSoCCtaSC/Start Yr Shares of Capacity Costs that are Soft Costs.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jeff-nonadmin\CodeRepositories\eps-us\InputData\endo-learn\SYSoCCtaSC\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\olivia\Dropbox (Energy Innovation)\Documents\EPS_Models by Region\United States\Model\InputData\endo-learn\SYSoCCtaSC\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{441BA37F-16B0-4405-B919-798EEE889669}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7FD0D10E-B959-477B-AADE-B0497EA8FE23}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="5610" yWindow="240" windowWidth="13328" windowHeight="9893" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="About" sheetId="1" r:id="rId1"/>
@@ -173,9 +173,6 @@
     <t>NREL</t>
   </si>
   <si>
-    <t>U.S. Solar Photovoltaic System Cost Benchmark: Q1 2017</t>
-  </si>
-  <si>
     <t>Page 13, Figure 2-8</t>
   </si>
   <si>
@@ -288,6 +285,9 @@
   </si>
   <si>
     <t>SYSoCCtaSC Start Year Share of Distributed Solar Costs that are Soft Costs</t>
+  </si>
+  <si>
+    <t>U.S. Solar Photovoltaic System Cost Benchmark: Q1 2018</t>
   </si>
 </sst>
 </file>
@@ -670,24 +670,26 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:B38"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C23" sqref="C23"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="2" max="2" width="61.42578125" customWidth="1"/>
+    <col min="2" max="2" width="61.3984375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A1" s="1" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A2" s="1" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A4" s="1" t="s">
         <v>0</v>
       </c>
@@ -695,144 +697,144 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.45">
       <c r="B5" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.45">
       <c r="B6" s="11">
         <v>2015</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.45">
       <c r="B7" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.45">
       <c r="B8" s="12" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.45">
       <c r="B9" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.45">
       <c r="B11" s="4" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.45">
       <c r="B12" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.45">
       <c r="B13" s="11">
         <v>2015</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:2" x14ac:dyDescent="0.45">
       <c r="B14" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.45">
       <c r="B15" s="12" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.45">
       <c r="B17" s="4" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:2" x14ac:dyDescent="0.45">
       <c r="B18" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:2" x14ac:dyDescent="0.45">
       <c r="B19" s="11">
-        <v>2017</v>
-      </c>
-    </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+        <v>2018</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.45">
       <c r="B20" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.45">
       <c r="B21" s="12" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:2" x14ac:dyDescent="0.45">
       <c r="B22" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A24" s="1" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A25" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A26" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A28" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A25" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A26" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A28" t="s">
+    <row r="29" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A29" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A29" t="s">
+    <row r="30" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A30" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A30" t="s">
+    <row r="32" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A32" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A32" t="s">
+    <row r="33" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A33" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="33" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A33" t="s">
+    <row r="34" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A34" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="34" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A34" t="s">
+    <row r="36" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A36" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="36" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A36" t="s">
+    <row r="37" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A37" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="37" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A37" t="s">
+    <row r="38" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A38" t="s">
         <v>60</v>
-      </c>
-    </row>
-    <row r="38" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A38" t="s">
-        <v>61</v>
       </c>
     </row>
   </sheetData>
@@ -850,23 +852,25 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:C73"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView topLeftCell="A58" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="A74" sqref="A74"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="28.140625" customWidth="1"/>
+    <col min="1" max="1" width="28.1328125" customWidth="1"/>
     <col min="2" max="2" width="26" customWidth="1"/>
-    <col min="3" max="3" width="19.140625" customWidth="1"/>
+    <col min="3" max="3" width="19.1328125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A1" s="6" t="s">
         <v>1</v>
       </c>
       <c r="B1" s="7"/>
       <c r="C1" s="7"/>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A3" s="4" t="s">
         <v>2</v>
       </c>
@@ -877,7 +881,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A4" t="s">
         <v>5</v>
       </c>
@@ -888,7 +892,7 @@
         <v>0.15</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A5" t="s">
         <v>5</v>
       </c>
@@ -899,7 +903,7 @@
         <v>0.37</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A6" t="s">
         <v>5</v>
       </c>
@@ -910,7 +914,7 @@
         <v>0.16</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A7" t="s">
         <v>6</v>
       </c>
@@ -921,7 +925,7 @@
         <v>0.04</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A8" t="s">
         <v>6</v>
       </c>
@@ -932,7 +936,7 @@
         <v>0.03</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A9" t="s">
         <v>6</v>
       </c>
@@ -943,7 +947,7 @@
         <v>0.03</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A10" t="s">
         <v>6</v>
       </c>
@@ -954,7 +958,7 @@
         <v>0.03</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A11" t="s">
         <v>6</v>
       </c>
@@ -965,7 +969,7 @@
         <v>0.08</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A12" t="s">
         <v>6</v>
       </c>
@@ -976,7 +980,7 @@
         <v>0.02</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A13" t="s">
         <v>6</v>
       </c>
@@ -987,7 +991,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A14" t="s">
         <v>20</v>
       </c>
@@ -998,7 +1002,7 @@
         <v>0.03</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A15" t="s">
         <v>20</v>
       </c>
@@ -1009,30 +1013,30 @@
         <v>0.06</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A18" s="1" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A19" s="10">
         <f>SUM(C12:C15,C7:C10)</f>
         <v>0.24</v>
       </c>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A22" s="6" t="s">
         <v>21</v>
       </c>
       <c r="B22" s="7"/>
       <c r="C22" s="7"/>
     </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A24" s="1" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A25" s="4" t="s">
         <v>3</v>
       </c>
@@ -1040,7 +1044,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A26" t="s">
         <v>23</v>
       </c>
@@ -1048,7 +1052,7 @@
         <v>0.31</v>
       </c>
     </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A27" t="s">
         <v>13</v>
       </c>
@@ -1056,7 +1060,7 @@
         <v>0.32</v>
       </c>
     </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A28" t="s">
         <v>24</v>
       </c>
@@ -1064,7 +1068,7 @@
         <v>0.28000000000000003</v>
       </c>
     </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A29" t="s">
         <v>25</v>
       </c>
@@ -1072,7 +1076,7 @@
         <v>0.02</v>
       </c>
     </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A30" t="s">
         <v>15</v>
       </c>
@@ -1080,7 +1084,7 @@
         <v>0.03</v>
       </c>
     </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A31" t="s">
         <v>26</v>
       </c>
@@ -1088,7 +1092,7 @@
         <v>0.04</v>
       </c>
     </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A32" t="s">
         <v>27</v>
       </c>
@@ -1096,10 +1100,10 @@
         <v>0.01</v>
       </c>
     </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:2" x14ac:dyDescent="0.45">
       <c r="B33" s="3"/>
     </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A34" t="s">
         <v>29</v>
       </c>
@@ -1107,7 +1111,7 @@
         <v>0.3</v>
       </c>
     </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A35" t="s">
         <v>30</v>
       </c>
@@ -1115,16 +1119,16 @@
         <v>0.7</v>
       </c>
     </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:2" x14ac:dyDescent="0.45">
       <c r="B36" s="3"/>
     </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A37" s="1" t="s">
         <v>19</v>
       </c>
       <c r="B37" s="3"/>
     </row>
-    <row r="38" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A38" s="9">
         <f>B35*SUM(B29:B32,B27)</f>
         <v>0.29399999999999998</v>
@@ -1133,15 +1137,15 @@
         <v>31</v>
       </c>
     </row>
-    <row r="39" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:2" x14ac:dyDescent="0.45">
       <c r="B39" s="3"/>
     </row>
-    <row r="41" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A41" s="1" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="42" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A42" s="4" t="s">
         <v>3</v>
       </c>
@@ -1149,7 +1153,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="43" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A43" t="s">
         <v>23</v>
       </c>
@@ -1157,7 +1161,7 @@
         <v>0.28000000000000003</v>
       </c>
     </row>
-    <row r="44" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A44" t="s">
         <v>13</v>
       </c>
@@ -1165,7 +1169,7 @@
         <v>0.21</v>
       </c>
     </row>
-    <row r="45" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A45" t="s">
         <v>24</v>
       </c>
@@ -1173,7 +1177,7 @@
         <v>0.43</v>
       </c>
     </row>
-    <row r="46" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A46" t="s">
         <v>25</v>
       </c>
@@ -1181,7 +1185,7 @@
         <v>0.02</v>
       </c>
     </row>
-    <row r="47" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A47" t="s">
         <v>15</v>
       </c>
@@ -1189,7 +1193,7 @@
         <v>0.02</v>
       </c>
     </row>
-    <row r="48" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A48" t="s">
         <v>26</v>
       </c>
@@ -1197,7 +1201,7 @@
         <v>0.02</v>
       </c>
     </row>
-    <row r="49" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A49" t="s">
         <v>27</v>
       </c>
@@ -1205,7 +1209,7 @@
         <v>0.02</v>
       </c>
     </row>
-    <row r="51" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A51" t="s">
         <v>29</v>
       </c>
@@ -1213,7 +1217,7 @@
         <v>0.3</v>
       </c>
     </row>
-    <row r="52" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A52" t="s">
         <v>30</v>
       </c>
@@ -1221,13 +1225,13 @@
         <v>0.7</v>
       </c>
     </row>
-    <row r="54" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A54" s="1" t="s">
         <v>19</v>
       </c>
       <c r="B54" s="3"/>
     </row>
-    <row r="55" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A55" s="9">
         <f>B52*SUM(B46:B49,B44)</f>
         <v>0.20299999999999999</v>
@@ -1236,25 +1240,25 @@
         <v>31</v>
       </c>
     </row>
-    <row r="57" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A57" s="1" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="58" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A58" s="10">
         <f>AVERAGE(A38,A55)</f>
         <v>0.2485</v>
       </c>
     </row>
-    <row r="61" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A61" s="6" t="s">
         <v>33</v>
       </c>
       <c r="B61" s="6"/>
       <c r="C61" s="6"/>
     </row>
-    <row r="63" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A63" s="1" t="s">
         <v>34</v>
       </c>
@@ -1262,54 +1266,54 @@
         <v>35</v>
       </c>
     </row>
-    <row r="64" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A64" t="s">
         <v>36</v>
       </c>
       <c r="B64" s="3">
-        <v>0.68</v>
-      </c>
-    </row>
-    <row r="65" spans="1:2" x14ac:dyDescent="0.25">
+        <v>0.63</v>
+      </c>
+    </row>
+    <row r="65" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A65" t="s">
         <v>37</v>
       </c>
       <c r="B65" s="3">
-        <v>0.59</v>
-      </c>
-    </row>
-    <row r="66" spans="1:2" x14ac:dyDescent="0.25">
+        <v>0.56000000000000005</v>
+      </c>
+    </row>
+    <row r="66" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A66" t="s">
         <v>38</v>
       </c>
       <c r="B66" s="3">
-        <v>0.41</v>
-      </c>
-    </row>
-    <row r="68" spans="1:2" x14ac:dyDescent="0.25">
+        <v>0.35</v>
+      </c>
+    </row>
+    <row r="68" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A68" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="69" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A69" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="70" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A70" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="72" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A72" s="1" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="73" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A73" s="8">
         <f>B66</f>
-        <v>0.41</v>
+        <v>0.35</v>
       </c>
     </row>
   </sheetData>
@@ -1324,147 +1328,147 @@
   </sheetPr>
   <dimension ref="A1:B17"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="29.5703125" customWidth="1"/>
-    <col min="2" max="2" width="16.42578125" customWidth="1"/>
+    <col min="1" max="1" width="29.59765625" customWidth="1"/>
+    <col min="2" max="2" width="16.3984375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" ht="45" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" ht="28.5" x14ac:dyDescent="0.45">
       <c r="B1" s="15" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A2" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B2" s="13">
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A3" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B3" s="13">
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A4" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B4" s="13">
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A5" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B5" s="13">
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A6" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B6" s="14">
         <f>Data!A19</f>
         <v>0.24</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A7" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B7" s="14">
         <f>Data!A73</f>
-        <v>0.41</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+        <v>0.35</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A8" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B8" s="13">
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A9" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B9" s="13">
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A10" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B10" s="13">
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A11" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B11" s="13">
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A12" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B12" s="13">
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A13" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B13" s="13">
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A14" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B14" s="14">
         <f>Data!A58</f>
         <v>0.2485</v>
       </c>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A15" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B15">
         <f>B11</f>
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A16" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B16">
         <f>B11</f>
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A17" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B17">
         <f>B9</f>
@@ -1485,60 +1489,60 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="29.5703125" customWidth="1"/>
-    <col min="2" max="2" width="16.42578125" customWidth="1"/>
+    <col min="1" max="1" width="29.59765625" customWidth="1"/>
+    <col min="2" max="2" width="16.3984375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" ht="45" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" ht="28.5" x14ac:dyDescent="0.45">
       <c r="B1" s="15" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A2" t="s">
         <v>79</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>80</v>
       </c>
       <c r="B2" s="13">
         <f>AVERAGE(Data!B64:B65)</f>
-        <v>0.63500000000000001</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+        <v>0.59499999999999997</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.45">
       <c r="B3" s="13"/>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.45">
       <c r="B4" s="13"/>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.45">
       <c r="B5" s="13"/>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.45">
       <c r="B6" s="14"/>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.45">
       <c r="B7" s="14"/>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.45">
       <c r="B8" s="13"/>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.45">
       <c r="B9" s="13"/>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.45">
       <c r="B10" s="13"/>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.45">
       <c r="B11" s="13"/>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.45">
       <c r="B12" s="13"/>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.45">
       <c r="B13" s="13"/>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:2" x14ac:dyDescent="0.45">
       <c r="B14" s="14"/>
     </row>
   </sheetData>

</xml_diff>